<commit_message>
fix: custom config built with gnu toolchain is incompatible with clang. So remove it and rely on default bigconfig of SyzDirect
</commit_message>
<xml_diff>
--- a/examples/vfs_dedupe_file_range_v5.10/dedupe_file_range_v5.10_dataset.xlsx
+++ b/examples/vfs_dedupe_file_range_v5.10/dedupe_file_range_v5.10_dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">idx</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">2c85ebc57b3e1817b6ce1a6b703928e113a90442</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/src/SyzDirect/examples/vfs_dedupe_file_range_v5.10/v5.10-syzkaller-btrfs-xfs.config</t>
   </si>
 </sst>
 </file>
@@ -339,7 +336,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,9 +374,7 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>